<commit_message>
Updated Telemetry Sensor Addresses.xlsx
git-svn-id: svn+ssh://localhost/home/pcb/svn@600 265e18a8-33ca-405d-8757-c40a9e3cabe4
</commit_message>
<xml_diff>
--- a/B Bus/Tray Interconnects/Telemetry Sensor Addresses.xlsx
+++ b/B Bus/Tray Interconnects/Telemetry Sensor Addresses.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="116">
   <si>
     <t>Sensor</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t>0x102DA59B020800AA</t>
+  </si>
+  <si>
+    <t>0x1060C12C0208008C</t>
+  </si>
+  <si>
+    <t>0x1000962C0208008B</t>
   </si>
 </sst>
 </file>
@@ -742,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A6" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="C21" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -925,6 +931,9 @@
       <c r="D10" s="3" t="s">
         <v>70</v>
       </c>
+      <c r="E10" s="3" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="3">
@@ -1415,7 +1424,9 @@
       <c r="D41" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E41" s="3"/>
+      <c r="E41" s="3" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">

</xml_diff>

<commit_message>
Corrected T1.4 sensor address.
git-svn-id: svn+ssh://localhost/home/pcb/svn@604 265e18a8-33ca-405d-8757-c40a9e3cabe4
</commit_message>
<xml_diff>
--- a/B Bus/Tray Interconnects/Telemetry Sensor Addresses.xlsx
+++ b/B Bus/Tray Interconnects/Telemetry Sensor Addresses.xlsx
@@ -333,9 +333,6 @@
     <t>0x10D9919B0208009F</t>
   </si>
   <si>
-    <t>0x1088839B0208009F</t>
-  </si>
-  <si>
     <t>0x10BE8E9B020800CA</t>
   </si>
   <si>
@@ -364,6 +361,9 @@
   </si>
   <si>
     <t>0x1000962C0208008B</t>
+  </si>
+  <si>
+    <t>0x1088839B02080079</t>
   </si>
 </sst>
 </file>
@@ -748,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="C21" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="C1" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -844,7 +844,7 @@
         <v>65</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -863,7 +863,7 @@
         <v>66</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -881,7 +881,7 @@
         <v>67</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -898,7 +898,7 @@
         <v>68</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -915,7 +915,7 @@
         <v>69</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -932,7 +932,7 @@
         <v>70</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -949,7 +949,7 @@
         <v>71</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -966,7 +966,7 @@
         <v>72</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -983,7 +983,7 @@
         <v>73</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1000,7 +1000,7 @@
         <v>74</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1425,7 +1425,7 @@
         <v>101</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:5">

</xml_diff>

<commit_message>
Updated Telemetry Sensor Addresses.xlsx with new addresses.
git-svn-id: svn+ssh://localhost/home/pcb/svn@605 265e18a8-33ca-405d-8757-c40a9e3cabe4
</commit_message>
<xml_diff>
--- a/B Bus/Tray Interconnects/Telemetry Sensor Addresses.xlsx
+++ b/B Bus/Tray Interconnects/Telemetry Sensor Addresses.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="118">
   <si>
     <t>Sensor</t>
   </si>
@@ -87,30 +87,6 @@
     <t>0x10DE7B2C0208006A</t>
   </si>
   <si>
-    <t>0x10C91EA90208002F</t>
-  </si>
-  <si>
-    <t>0x106935A9020800FB</t>
-  </si>
-  <si>
-    <t>0x1093FDA8020800D5</t>
-  </si>
-  <si>
-    <t>0x103E1AA9020800C7</t>
-  </si>
-  <si>
-    <t>0x10DB18A902080086</t>
-  </si>
-  <si>
-    <t>0x1028E5A802080014</t>
-  </si>
-  <si>
-    <t>0x10B826A90208003A</t>
-  </si>
-  <si>
-    <t>0x104ACFA802080080</t>
-  </si>
-  <si>
     <t>RX1 RF Input Transistor</t>
   </si>
   <si>
@@ -141,9 +117,6 @@
     <t>TX1 Ground Plane</t>
   </si>
   <si>
-    <t>TX1 Multiplier Transistor</t>
-  </si>
-  <si>
     <t>TX2 RF Power Transistor</t>
   </si>
   <si>
@@ -153,9 +126,6 @@
     <t>TX2 Ground Plane</t>
   </si>
   <si>
-    <t>TX2 Multiplier Transistor</t>
-  </si>
-  <si>
     <t>RX Interconnect (SMD)</t>
   </si>
   <si>
@@ -189,18 +159,6 @@
     <t>Tray 2 Sensor 9</t>
   </si>
   <si>
-    <t>Tray 2 Sensor 10</t>
-  </si>
-  <si>
-    <t>Tray 2 Sensor 11</t>
-  </si>
-  <si>
-    <t>Tray 2 Sensor 12</t>
-  </si>
-  <si>
-    <t>Tray 2 Sensor 13</t>
-  </si>
-  <si>
     <t>UID</t>
   </si>
   <si>
@@ -261,15 +219,6 @@
     <t>T2.10</t>
   </si>
   <si>
-    <t>T2.11</t>
-  </si>
-  <si>
-    <t>T2.12</t>
-  </si>
-  <si>
-    <t>T2.13</t>
-  </si>
-  <si>
     <t>T3.1</t>
   </si>
   <si>
@@ -318,12 +267,6 @@
     <t>T5.7</t>
   </si>
   <si>
-    <t>T5.8</t>
-  </si>
-  <si>
-    <t>T5.9</t>
-  </si>
-  <si>
     <t>0x10C1969B02080034</t>
   </si>
   <si>
@@ -345,18 +288,6 @@
     <t>0x1029AA9B02080019</t>
   </si>
   <si>
-    <t>0x105E889B0208007F</t>
-  </si>
-  <si>
-    <t>0x105F9A9B020800B7</t>
-  </si>
-  <si>
-    <t>0x103E9D9B02080012</t>
-  </si>
-  <si>
-    <t>0x102DA59B020800AA</t>
-  </si>
-  <si>
     <t>0x1060C12C0208008C</t>
   </si>
   <si>
@@ -364,6 +295,81 @@
   </si>
   <si>
     <t>0x1088839B02080079</t>
+  </si>
+  <si>
+    <t>0x10857D8402080095</t>
+  </si>
+  <si>
+    <t>0x1097958402080044</t>
+  </si>
+  <si>
+    <t>0x10441F82020800A6</t>
+  </si>
+  <si>
+    <t>0x10A1978402080098</t>
+  </si>
+  <si>
+    <t>0x10BA798402080043</t>
+  </si>
+  <si>
+    <t>0x107A7C840208000E</t>
+  </si>
+  <si>
+    <t>Tray 2 Onboard Sensor</t>
+  </si>
+  <si>
+    <t>0x10407984020800FE</t>
+  </si>
+  <si>
+    <t>0x106F888402080007</t>
+  </si>
+  <si>
+    <t>0x10AE7A840208008A</t>
+  </si>
+  <si>
+    <t>0x10779084020800BF</t>
+  </si>
+  <si>
+    <t>0x10B97D8402080005</t>
+  </si>
+  <si>
+    <t>0x1013838402080092</t>
+  </si>
+  <si>
+    <t>0x10278784020800BC</t>
+  </si>
+  <si>
+    <t>0x10967A84020800C6</t>
+  </si>
+  <si>
+    <t>0x106A968402080032</t>
+  </si>
+  <si>
+    <t>0x104D8B8402080091</t>
+  </si>
+  <si>
+    <t>0x10FE818402080072</t>
+  </si>
+  <si>
+    <t>0x1074FF8102080019</t>
+  </si>
+  <si>
+    <t>0x10B9408202080064</t>
+  </si>
+  <si>
+    <t>0x108060810208006F</t>
+  </si>
+  <si>
+    <t>0x106E7E840208000A</t>
+  </si>
+  <si>
+    <t>0x10C37E840208001C</t>
+  </si>
+  <si>
+    <t>0x10E89584020800F8</t>
+  </si>
+  <si>
+    <t>Master Addresses</t>
   </si>
 </sst>
 </file>
@@ -446,8 +452,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E74" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E69" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:E69">
     <filterColumn colId="3"/>
   </autoFilter>
   <tableColumns count="5">
@@ -746,11 +752,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="C1" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="85" zoomScalePageLayoutView="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -771,7 +775,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -785,13 +789,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -802,13 +806,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -820,13 +824,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -838,13 +842,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -857,13 +861,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -875,13 +879,13 @@
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -892,13 +896,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -909,13 +913,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -926,13 +930,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -943,13 +947,13 @@
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -960,13 +964,13 @@
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -977,13 +981,13 @@
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -994,13 +998,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1011,12 +1015,14 @@
         <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="3"/>
+        <v>61</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3">
@@ -1026,12 +1032,14 @@
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3">
@@ -1041,12 +1049,14 @@
         <v>5</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="3"/>
+        <v>63</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3">
@@ -1056,12 +1066,14 @@
         <v>5</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3">
@@ -1071,12 +1083,14 @@
         <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3">
@@ -1086,10 +1100,10 @@
         <v>5</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="E20" s="3"/>
     </row>
@@ -1098,45 +1112,51 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="3"/>
+        <v>68</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" s="3"/>
+        <v>69</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3">
@@ -1146,13 +1166,13 @@
         <v>6</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1163,13 +1183,13 @@
         <v>6</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1180,13 +1200,13 @@
         <v>6</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1197,13 +1217,13 @@
         <v>6</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1214,13 +1234,13 @@
         <v>6</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>26</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1231,13 +1251,13 @@
         <v>6</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1245,16 +1265,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1262,16 +1282,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1279,16 +1299,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1299,12 +1319,14 @@
         <v>4</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E33" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3">
@@ -1314,12 +1336,14 @@
         <v>4</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E34" s="3"/>
+        <v>80</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3">
@@ -1329,12 +1353,14 @@
         <v>4</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E35" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3">
@@ -1344,119 +1370,49 @@
         <v>4</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E36" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="3">
-        <v>36</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="A37" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="3">
-        <v>37</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E38" s="3"/>
+      <c r="B38" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="3">
-        <v>38</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E39" s="3"/>
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="3">
-        <v>39</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E40" s="3"/>
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="3">
-        <v>40</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" t="s">
+      <c r="A41" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Tray 2 Onboard Sensor T2.10 address
git-svn-id: svn+ssh://localhost/home/pcb/svn@612 265e18a8-33ca-405d-8757-c40a9e3cabe4
</commit_message>
<xml_diff>
--- a/B Bus/Tray Interconnects/Telemetry Sensor Addresses.xlsx
+++ b/B Bus/Tray Interconnects/Telemetry Sensor Addresses.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="119">
   <si>
     <t>Sensor</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>Master Addresses</t>
+  </si>
+  <si>
+    <t>0x10F8469202080082</t>
   </si>
 </sst>
 </file>
@@ -754,7 +757,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="85" zoomScalePageLayoutView="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScale="115" zoomScaleNormal="85" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1105,7 +1110,9 @@
       <c r="D20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3">

</xml_diff>